<commit_message>
> It seems there is no effect of movements ...
</commit_message>
<xml_diff>
--- a/HOEMWORK_2.xlsx
+++ b/HOEMWORK_2.xlsx
@@ -42,10 +42,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,13 +84,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -102,6 +129,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Packets Dropped</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -116,11 +168,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -142,19 +194,112 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>number of packets</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CBK</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>COL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NRTE</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RET</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$4</c:f>
+              <c:f>Sheet1!$B$1:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -174,56 +319,22 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-2080044448"/>
-        <c:axId val="-2112752016"/>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="-2066033488"/>
+        <c:axId val="-2054241552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2080044448"/>
+        <c:axId val="-2066033488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -235,11 +346,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -266,34 +377,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2112752016"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="-2054241552"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112752016"/>
+        <c:axId val="-2054241552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -325,8 +421,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080044448"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="-2066033488"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -338,7 +433,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -447,7 +542,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -458,7 +553,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -471,11 +566,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -488,7 +583,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -504,7 +599,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -548,32 +643,70 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
@@ -585,33 +718,29 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -633,15 +762,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -656,15 +783,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -675,10 +802,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -694,14 +821,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -713,31 +840,24 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -746,17 +866,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -765,29 +884,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -795,6 +895,24 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -815,7 +933,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -823,7 +941,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -843,10 +961,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -863,11 +981,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -876,14 +994,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -913,8 +1030,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -937,14 +1054,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -953,20 +1064,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1250,41 +1361,41 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:B4"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>166</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B4" s="1">
         <v>38</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>